<commit_message>
update bom & readme
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwmag\Documents\C\rhythmcontroller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwmag\Documents\C\ergodash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EDD668-D03E-492A-9783-752FF1140FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80941A2A-E453-4452-94F7-A07F766FC13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{506A362A-19F2-45D6-B4FC-6327898CF8C7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -58,9 +58,6 @@
     <t>White LED</t>
   </si>
   <si>
-    <t>D00, D01, D02, D10, D11, D12, D20, D21, D22</t>
-  </si>
-  <si>
     <t>Kailh Red Switch Socket</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>C1-C10</t>
   </si>
   <si>
-    <t>R11-R13</t>
-  </si>
-  <si>
     <t>R1-R10</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t>6mm D shaft knob</t>
   </si>
   <si>
-    <t>1528-4958-ND</t>
-  </si>
-  <si>
     <t>6mm D shaft encoder w/ switch</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>initial</t>
   </si>
   <si>
-    <t>pcbs</t>
-  </si>
-  <si>
     <t>digikey parts rd 1</t>
   </si>
   <si>
@@ -193,9 +181,6 @@
     <t>(AliExpress) 1005003796855429</t>
   </si>
   <si>
-    <t>(AliExpress) 1005003977714274</t>
-  </si>
-  <si>
     <t>S0-S3, S5, S6</t>
   </si>
   <si>
@@ -223,20 +208,64 @@
     <t>Delvie's Plastics Translucent Cast</t>
   </si>
   <si>
-    <t>Delvie's Plastics The Pastels</t>
-  </si>
-  <si>
     <t>delvie's plastics order</t>
+  </si>
+  <si>
+    <t>R11-R14</t>
+  </si>
+  <si>
+    <t>D00 - D33</t>
+  </si>
+  <si>
+    <t>digikey round 3</t>
+  </si>
+  <si>
+    <t>(Amazon) B09MVJDRGD</t>
+  </si>
+  <si>
+    <t>https://kbdfans.com/products/mechanical-keyboard-low-profile-switches-kailh-pcb-socket-cpg135001s30?variant=39678407671947</t>
+  </si>
+  <si>
+    <t>jlcpcb - 1</t>
+  </si>
+  <si>
+    <t>jlcpcb - 2</t>
+  </si>
+  <si>
+    <t>amazon - keycaps</t>
+  </si>
+  <si>
+    <t>aliexpress - spacebars</t>
+  </si>
+  <si>
+    <t>primekb - stabilizers</t>
+  </si>
+  <si>
+    <t>On Order</t>
+  </si>
+  <si>
+    <t>Sets (incl. On Order)</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -259,16 +288,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -578,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44686417-63E4-4AF5-BB45-7CFF55B6C5A1}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,13 +674,14 @@
     <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="5.140625" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="16" max="16" width="25" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -611,36 +695,45 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -653,77 +746,91 @@
         <v>0.25</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>40</v>
       </c>
-      <c r="H2">
-        <f t="shared" ref="H2:H4" si="0">FLOOR(G2/D2, 1)</f>
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2">
+      <c r="I2">
+        <f>FLOOR((H2 + G2)/D2, 1)</f>
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J4" si="0">FLOOR(H2/D2, 1)</f>
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2">
         <f>SUM(F:F)</f>
-        <v>37.939166666666665</v>
-      </c>
-      <c r="N2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2">
+        <v>42.68333333333333</v>
+      </c>
+      <c r="P2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F4" si="1">D3*E3</f>
-        <v>0.13500000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>12</v>
       </c>
-      <c r="H3">
+      <c r="I3">
+        <f t="shared" ref="I3:I19" si="2">FLOOR((H3 + G3)/D3, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="J3">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3">
-        <f>MIN(H:H)</f>
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3">
+        <f>MIN(J:J)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3">
         <f>500-18.81</f>
         <v>481.19</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -736,100 +843,121 @@
         <v>0.94</v>
       </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>14</v>
       </c>
-      <c r="H4">
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4">
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4">
         <f>481.19-73.84</f>
         <v>407.35</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>0.11</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F15" si="2">D5*E5</f>
-        <v>0.99</v>
+        <f t="shared" ref="F5:F15" si="3">D5*E5</f>
+        <v>1.76</v>
       </c>
       <c r="G5">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H19" si="3">FLOOR(G5/D5, 1)</f>
-        <v>4</v>
-      </c>
-      <c r="N5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <f>FLOOR(H5/D5, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5">
         <f>407.35-35.82</f>
         <v>371.53000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
       <c r="E6">
-        <f>4.95/20</f>
-        <v>0.2475</v>
+        <f>33/500</f>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
-        <v>1.7324999999999999</v>
+        <f t="shared" si="3"/>
+        <v>0.46200000000000002</v>
       </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>13</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>46</v>
-      </c>
-      <c r="O6">
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J19" si="4">FLOOR(H6/D6, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6">
         <f>371.54-8.65</f>
         <v>362.89000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -839,33 +967,40 @@
         <v>0.31657142857142856</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.2159999999999997</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O7">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7">
         <f>362.89-41.19</f>
         <v>321.7</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -874,54 +1009,83 @@
         <v>0.188</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.88</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q8">
+        <f>321.7-23.7</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f>12.92/5</f>
+        <v>2.5840000000000001</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>2.5840000000000001</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q9">
+        <f>298-30.14</f>
+        <v>267.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0.99</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>0.99</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
+      <c r="C10" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -931,55 +1095,83 @@
         <v>3.4619999999999997</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.4619999999999997</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q10">
+        <f>267.86 - 8.64</f>
+        <v>259.22000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D11">
         <v>7</v>
       </c>
       <c r="E11">
-        <f>2.58/20</f>
-        <v>0.129</v>
+        <f>8.64/20</f>
+        <v>0.43200000000000005</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
-        <v>0.90300000000000002</v>
+        <f t="shared" si="3"/>
+        <v>3.0240000000000005</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q11">
+        <f>259.22 - 12.92</f>
+        <v>246.30000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -988,26 +1180,40 @@
         <v>11.95</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.95</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="P12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q12">
+        <f>246.3-17.31</f>
+        <v>228.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1016,26 +1222,33 @@
         <v>0.71599999999999997</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.71599999999999997</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1044,23 +1257,30 @@
         <v>1.88</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.88</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1070,26 +1290,33 @@
         <v>2.6399999999999997</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.6399999999999997</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1099,55 +1326,69 @@
         <v>2.6346666666666669</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16" si="4">D16*E16</f>
+        <f t="shared" ref="F16" si="5">D16*E16</f>
         <v>2.6346666666666669</v>
       </c>
       <c r="G16">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <f>9.2/8</f>
-        <v>1.1499999999999999</v>
+        <f>39.52/15</f>
+        <v>2.6346666666666669</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F19" si="5">D17*E17</f>
-        <v>1.1499999999999999</v>
+        <f t="shared" ref="F17:F19" si="6">D17*E17</f>
+        <v>2.6346666666666669</v>
       </c>
       <c r="G17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1156,26 +1397,33 @@
         <v>1.47</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.47</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19">
         <v>20</v>
@@ -1184,18 +1432,39 @@
         <v>0.1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H19">
-        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J2:J19">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I19">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{030239F7-8DAB-48B5-A03B-4411BEF4BDCF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>